<commit_message>
Including API requests exercises
</commit_message>
<xml_diff>
--- a/Simpson_best_chapters.xlsx
+++ b/Simpson_best_chapters.xlsx
@@ -92,79 +92,79 @@
     <t>25</t>
   </si>
   <si>
-    <t>1. The Itchy &amp; Scratchy &amp; Poochie Show</t>
-  </si>
-  <si>
-    <t>2. Homie the Clown</t>
-  </si>
-  <si>
-    <t>3. Bart Gets an Elephant</t>
-  </si>
-  <si>
-    <t>4. Homer Goes to College</t>
-  </si>
-  <si>
-    <t>5. Bart’s Inner Child</t>
-  </si>
-  <si>
-    <t>6. Rosebud</t>
-  </si>
-  <si>
-    <t>7. Homer’s Enemy</t>
-  </si>
-  <si>
-    <t>8. Homer vs. the Eighteenth Amendment</t>
-  </si>
-  <si>
-    <t>9. A Milhouse Divided</t>
-  </si>
-  <si>
-    <t>10. Marge vs. the Monorail</t>
-  </si>
-  <si>
-    <t>11. You Only Move Twice</t>
-  </si>
-  <si>
-    <t>12. Homer Badman</t>
-  </si>
-  <si>
-    <t>13. Grade School Confidential</t>
-  </si>
-  <si>
-    <t>14. Realty Bites</t>
-  </si>
-  <si>
-    <t>15. Last Exit to Springfield</t>
-  </si>
-  <si>
-    <t>16. The Last Temptation of Homer</t>
-  </si>
-  <si>
-    <t>17. The Boy Who Knew Too Much</t>
-  </si>
-  <si>
-    <t>18. King-Size Homer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19. The Cartridge Family </t>
-  </si>
-  <si>
-    <t>20. Deep Space Homer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21. Homer at the Bat </t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. Team Homer </t>
-  </si>
-  <si>
-    <t>23. Lisa’s Rival</t>
-  </si>
-  <si>
-    <t>24. All’s Fair in Oven War</t>
-  </si>
-  <si>
-    <t>25. Homer the Vigilante</t>
+    <t>The Itchy &amp; Scratchy &amp; Poochie Show</t>
+  </si>
+  <si>
+    <t>Homie the Clown</t>
+  </si>
+  <si>
+    <t>Bart Gets an Elephant</t>
+  </si>
+  <si>
+    <t>Homer Goes to College</t>
+  </si>
+  <si>
+    <t>Bart’s Inner Child</t>
+  </si>
+  <si>
+    <t>Rosebud</t>
+  </si>
+  <si>
+    <t>Homer’s Enemy</t>
+  </si>
+  <si>
+    <t>Homer vs. the Eighteenth Amendment</t>
+  </si>
+  <si>
+    <t>A Milhouse Divided</t>
+  </si>
+  <si>
+    <t>Marge vs. the Monorail</t>
+  </si>
+  <si>
+    <t>You Only Move Twice</t>
+  </si>
+  <si>
+    <t>Homer Badman</t>
+  </si>
+  <si>
+    <t>Grade School Confidential</t>
+  </si>
+  <si>
+    <t>Realty Bites</t>
+  </si>
+  <si>
+    <t>Last Exit to Springfield</t>
+  </si>
+  <si>
+    <t>The Last Temptation of Homer</t>
+  </si>
+  <si>
+    <t>The Boy Who Knew Too Much</t>
+  </si>
+  <si>
+    <t>King-Size Homer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cartridge Family </t>
+  </si>
+  <si>
+    <t>Deep Space Homer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homer at the Bat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team Homer </t>
+  </si>
+  <si>
+    <t>Lisa’s Rival</t>
+  </si>
+  <si>
+    <t>All’s Fair in Oven War</t>
+  </si>
+  <si>
+    <t>Homer the Vigilante</t>
   </si>
 </sst>
 </file>

</xml_diff>